<commit_message>
updated main, first commit sunpharma simulations
</commit_message>
<xml_diff>
--- a/input/input_data.xlsx
+++ b/input/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa\Desktop\Github\Project\GRANULE\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B51B1F-1E96-460E-820D-D2AA7903A546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C951EEFB-2637-4A9D-AB03-EB6F67C4CAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6516" yWindow="48" windowWidth="11640" windowHeight="12312" xr2:uid="{4594D694-8109-428A-85DC-383A96E259B8}"/>
+    <workbookView xWindow="1536" yWindow="48" windowWidth="11640" windowHeight="12312" activeTab="1" xr2:uid="{4594D694-8109-428A-85DC-383A96E259B8}"/>
   </bookViews>
   <sheets>
     <sheet name="design input" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +91,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -118,11 +126,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -445,19 +454,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3E30C5-DF56-4F1A-A01E-D919CA2EC5AB}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -465,67 +474,67 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3">
         <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4">
         <v>4.05</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8">
         <v>2.1</v>
       </c>
@@ -546,79 +555,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F97F670-4122-4351-BC34-50B30D00AD97}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="F3">
         <v>0.23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
granule model complete v0
</commit_message>
<xml_diff>
--- a/input/input_data.xlsx
+++ b/input/input_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa\Desktop\Github\Project\GRANULE\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa\Desktop\Github\GRANULE\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7712B4-45AE-459B-95FD-39AD1E5DD0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7366E056-20D1-476A-B991-33AB0506E64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1032" windowWidth="21600" windowHeight="11328" xr2:uid="{4594D694-8109-428A-85DC-383A96E259B8}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="21600" windowHeight="11328" activeTab="1" xr2:uid="{4594D694-8109-428A-85DC-383A96E259B8}"/>
   </bookViews>
   <sheets>
-    <sheet name="design input" sheetId="1" r:id="rId1"/>
-    <sheet name="influent input" sheetId="2" r:id="rId2"/>
+    <sheet name="influent input" sheetId="2" r:id="rId1"/>
+    <sheet name="design input" sheetId="1" r:id="rId2"/>
+    <sheet name="kinetic coefficients" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Design data of reactor</t>
   </si>
@@ -78,6 +79,27 @@
   </si>
   <si>
     <t>Substrate/ biomass working ratio [-]</t>
+  </si>
+  <si>
+    <t>Simulation time [days]</t>
+  </si>
+  <si>
+    <t>Decay constant [h]:</t>
+  </si>
+  <si>
+    <t>B0    [LCH4/g COD added]:</t>
+  </si>
+  <si>
+    <t>Half saturation constant (Monod kinetics) [kg/m3]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insert n° CSTR for simulation: </t>
+  </si>
+  <si>
+    <t>Discretization number:</t>
+  </si>
+  <si>
+    <t>Reactor model behaviour:</t>
   </si>
 </sst>
 </file>
@@ -129,24 +151,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -162,7 +186,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -457,96 +481,254 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3E30C5-DF56-4F1A-A01E-D919CA2EC5AB}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F97F670-4122-4351-BC34-50B30D00AD97}">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4">
+        <f>F3/F12</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5">
+        <v>1.5</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12">
+        <f>0.23/2</f>
+        <v>0.115</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3E30C5-DF56-4F1A-A01E-D919CA2EC5AB}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4">
-        <v>4.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+        <f>(E3*4/3.14/E5)^0.5</f>
+        <v>7.9808688446762206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
       <c r="E5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="E6">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
       <c r="E7">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+        <f>E8*E4</f>
+        <v>23.942606534028663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
       <c r="E8">
-        <v>2.1</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14">
+        <f>1-(1.03*E8^(1.11)*0.009^(1/E11))/(1.03*E8^(1.11))</f>
+        <v>0.1453110608102739</v>
+      </c>
+      <c r="G14" s="4" t="str">
+        <f>IF(E14&gt;0.75,"CSTR",IF(E14&lt;0.15, "PFR", "HYBRID APPROACH"))</f>
+        <v>PFR</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A14:D14"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A1:D1"/>
@@ -559,110 +741,82 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F97F670-4122-4351-BC34-50B30D00AD97}">
-  <dimension ref="A1:I12"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8B70D2-C399-4AD0-AAA2-1CA648D83B0E}">
+  <dimension ref="A2:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
       <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
       <c r="F5">
-        <v>1.5</v>
-      </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12">
-        <f>0.23/2</f>
-        <v>0.115</v>
-      </c>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:E2"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>